<commit_message>
se cambio la interfaz
</commit_message>
<xml_diff>
--- a/proyectoUI/resultado.xlsx
+++ b/proyectoUI/resultado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>NATURALEZA</t>
+          <t>Unnamed: 1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -471,15 +471,25 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>COMENTARIOS DCP</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>COMENTARIOS CONTADOR</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>InputText</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Clasificación_Predicha</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>PR_PNR_Predicho</t>
         </is>
@@ -488,7 +498,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>102-01</t>
+          <t>101-01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -498,32 +508,34 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>bancos nacionales</t>
+          <t>cajayefectivo</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>862806.3</v>
+        <v>1000</v>
       </c>
       <c r="E2" t="n">
-        <v>40927858.15</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>37087836.94</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>4702827.51</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>CUENTA 102-01 NOMBRE bancos nacionales</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
+        <v>1000</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>CUENTA 101-01 NOMBRE cajayefectivo</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>Efectivo y equivalentes de efectivo</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -542,32 +554,34 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>bbva</t>
+          <t>hsbcmxn</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>723920.17</v>
+        <v>71869.14999999999</v>
       </c>
       <c r="E3" t="n">
-        <v>33949595.1</v>
+        <v>408515.97</v>
       </c>
       <c r="F3" t="n">
-        <v>30143565.74</v>
+        <v>345398.78</v>
       </c>
       <c r="G3" t="n">
-        <v>4529949.53</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>CUENTA 102-01-01 NOMBRE bbva</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+        <v>134986.34</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>CUENTA 102-01-01 NOMBRE hsbcmxn</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>Efectivo y equivalentes de efectivo</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -586,32 +600,34 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>bbva usd</t>
+          <t>hsbcusd</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>123205.02</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>33803.83</v>
+        <v>1057420.78</v>
       </c>
       <c r="F4" t="n">
-        <v>9440.23</v>
+        <v>923321.55</v>
       </c>
       <c r="G4" t="n">
-        <v>147568.62</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>CUENTA 102-01-02 NOMBRE bbva usd</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
+        <v>134099.23</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>CUENTA 102-01-02 NOMBRE hsbcusd</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>Efectivo y equivalentes de efectivo</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -634,28 +650,30 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>15681.11</v>
+        <v>7819.83</v>
       </c>
       <c r="E5" t="n">
-        <v>6944459.22</v>
+        <v>107718.67</v>
       </c>
       <c r="F5" t="n">
-        <v>6934830.97</v>
+        <v>115586.18</v>
       </c>
       <c r="G5" t="n">
-        <v>25309.36</v>
-      </c>
-      <c r="H5" t="inlineStr">
+        <v>-47.68</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
         <is>
           <t>CUENTA 102-01-03 NOMBRE stripe</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>Efectivo y equivalentes de efectivo</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -674,32 +692,34 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>clientes nacionales</t>
+          <t>clientesnacionales</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>408134.72</v>
+        <v>94995.42999999999</v>
       </c>
       <c r="E6" t="n">
-        <v>14430369.23</v>
+        <v>349883.44</v>
       </c>
       <c r="F6" t="n">
-        <v>13966247.41</v>
+        <v>322507.44</v>
       </c>
       <c r="G6" t="n">
-        <v>872256.54</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>CUENTA 105-01 NOMBRE clientes nacionales</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Clientes</t>
-        </is>
-      </c>
+        <v>122371.43</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
+        <is>
+          <t>CUENTA 105-01 NOMBRE clientesnacionales</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Inventarios</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -718,32 +738,34 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>iva a favor</t>
+          <t>ivaafavor</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>9037</v>
+        <v>35291.02</v>
       </c>
       <c r="E7" t="n">
-        <v>132190.88</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>141227.88</v>
+        <v>35291.02</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>CUENTA 113-01 NOMBRE iva a favor</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Impuesto por recuperar</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
+        <is>
+          <t>CUENTA 113-01 NOMBRE ivaafavor</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Inventarios</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -752,7 +774,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>113-07</t>
+          <t>118-01</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -762,32 +784,34 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>pago de lo indebido</t>
+          <t>ivaacreditablepagado</t>
         </is>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>397.53</v>
+        <v>6831.27</v>
       </c>
       <c r="F8" t="n">
-        <v>334.53</v>
+        <v>6831.27</v>
       </c>
       <c r="G8" t="n">
-        <v>63</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>CUENTA 113-07 NOMBRE pago de lo indebido</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Impuesto por recuperar</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
+        <is>
+          <t>CUENTA 118-01 NOMBRE ivaacreditablepagado</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Inventarios</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -796,7 +820,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>114-01</t>
+          <t>119-01</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -806,32 +830,34 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>pagos provisionales de isr</t>
+          <t>ivapendientedepago</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>5218.97</v>
       </c>
       <c r="E9" t="n">
-        <v>6418</v>
+        <v>7067.33</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>6831.27</v>
       </c>
       <c r="G9" t="n">
-        <v>6418</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>CUENTA 114-01 NOMBRE pagos provisionales de isr</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Impuestos por pagar</t>
-        </is>
-      </c>
+        <v>5455.03</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
+        <is>
+          <t>CUENTA 119-01 NOMBRE ivapendientedepago</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Inventarios</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -840,7 +866,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>118-01</t>
+          <t>120-02</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -850,32 +876,34 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>iva acreditable pagado</t>
+          <t>anticipoaproveedoresextranjero</t>
         </is>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>1379594.96</v>
+        <v>90435.67999999999</v>
       </c>
       <c r="F10" t="n">
-        <v>1379594.96</v>
+        <v>90435.67999999999</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>CUENTA 118-01 NOMBRE iva acreditable pagado</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Impuesto por recuperar</t>
-        </is>
-      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
+        <is>
+          <t>CUENTA 120-02 NOMBRE anticipoaproveedoresextranjero</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Inventarios</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -884,7 +912,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>119-01</t>
+          <t>121-01-01</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -894,32 +922,34 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>iva pendiente de pago</t>
+          <t>ventasretenidas</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>87505.24000000001</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>1422740.86</v>
+        <v>8256.459999999999</v>
       </c>
       <c r="F11" t="n">
-        <v>1416713.36</v>
+        <v>8256.459999999999</v>
       </c>
       <c r="G11" t="n">
-        <v>93532.74000000001</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>CUENTA 119-01 NOMBRE iva pendiente de pago</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Impuesto por recuperar</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
+        <is>
+          <t>CUENTA 121-01-01 NOMBRE ventasretenidas</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Efectivo y equivalentes de efectivo</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -928,7 +958,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>120-01</t>
+          <t>121-01-02</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -938,32 +968,34 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>anticipo a proveedores nacional</t>
+          <t>ventasretenidasfarmacia</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>16287.69</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>806.53</v>
+        <v>107718.67</v>
       </c>
       <c r="F12" t="n">
-        <v>16287.69</v>
+        <v>107718.67</v>
       </c>
       <c r="G12" t="n">
-        <v>806.53</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>CUENTA 120-01 NOMBRE anticipo a proveedores nacional</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Anticipo a proveedores</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
+        <is>
+          <t>CUENTA 121-01-02 NOMBRE ventasretenidasfarmacia</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Efectivo y equivalentes de efectivo</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -972,7 +1004,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>121-01</t>
+          <t>121-01-03</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -982,32 +1014,34 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>otros activos a corto plazo</t>
+          <t>stripetraspaso</t>
         </is>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>107401.64</v>
+        <v>14258.4</v>
       </c>
       <c r="F13" t="n">
-        <v>107401.64</v>
+        <v>14258.4</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>CUENTA 121-01 NOMBRE otros activos a corto plazo</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Activos intangibles</t>
-        </is>
-      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
+        <is>
+          <t>CUENTA 121-01-03 NOMBRE stripetraspaso</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Efectivo y equivalentes de efectivo</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -1016,42 +1050,44 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>121-01-001</t>
+          <t>201-01</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>propinas x cobrar</t>
+          <t>proveedoresnacionales</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>32283.29</v>
       </c>
       <c r="E14" t="n">
-        <v>1072046.58</v>
+        <v>49526.69</v>
       </c>
       <c r="F14" t="n">
-        <v>758690.41</v>
+        <v>51238.17</v>
       </c>
       <c r="G14" t="n">
-        <v>313356.17</v>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>CUENTA 121-01-001 NOMBRE propinas x cobrar</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Efectivo y equivalentes de efectivo</t>
-        </is>
-      </c>
+        <v>33994.77</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
+        <is>
+          <t>CUENTA 201-01 NOMBRE proveedoresnacionales</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Acreedores diversos</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -1060,42 +1096,44 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>184-02</t>
+          <t>206-01</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>depósitos de arrendamiento de bienes inmuebles</t>
+          <t>anticipodeclientenacional</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1600</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>53806.55</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>53806.55</v>
       </c>
       <c r="G15" t="n">
-        <v>1600</v>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>CUENTA 184-02 NOMBRE depósitos de arrendamiento de bienes inmuebles</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Anticipo de clientes</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
+        <is>
+          <t>CUENTA 206-01 NOMBRE anticipodeclientenacional</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Activos intangibles</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -1104,7 +1142,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>201-01</t>
+          <t>208-01</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1114,32 +1152,34 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>proveedores nacionales</t>
+          <t>ivatrasladadocobrado</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>966676.49</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>10639503.26</v>
+        <v>48788.18</v>
       </c>
       <c r="F16" t="n">
-        <v>10625046.47</v>
+        <v>48788.18</v>
       </c>
       <c r="G16" t="n">
-        <v>952219.7</v>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>CUENTA 201-01 NOMBRE proveedores nacionales</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>Proveedores</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
+        <is>
+          <t>CUENTA 208-01 NOMBRE ivatrasladadocobrado</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Acreedores diversos</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -1148,7 +1188,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>201-04</t>
+          <t>209-01</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1158,32 +1198,34 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>proveedores extranjeros parte relacionada</t>
+          <t>ivatrasladadonocobrado</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>13102.82</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>44483.78</v>
       </c>
       <c r="F17" t="n">
-        <v>3798291</v>
+        <v>48259.78</v>
       </c>
       <c r="G17" t="n">
-        <v>3798291</v>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>CUENTA 201-04 NOMBRE proveedores extranjeros parte relacionada</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Proveedores</t>
-        </is>
-      </c>
+        <v>16878.82</v>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
+        <is>
+          <t>CUENTA 209-01 NOMBRE ivatrasladadonocobrado</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Acreedores diversos</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -1192,7 +1234,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>202-03</t>
+          <t>210-01</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1202,32 +1244,34 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>documentos y cuentas por pagar a corto plazo nacional</t>
+          <t>provisióndesueldosysalariosporpagar</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>62912.14</v>
+        <v>87436.86</v>
       </c>
       <c r="E18" t="n">
-        <v>18493317.67</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>19034733.53</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>604328</v>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>CUENTA 202-03 NOMBRE documentos y cuentas por pagar a corto plazo nacional</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>Cuentas y documentos por pagar</t>
-        </is>
-      </c>
+        <v>87436.86</v>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
+        <is>
+          <t>CUENTA 210-01 NOMBRE provisióndesueldosysalariosporpagar</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Inventarios</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -1236,7 +1280,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>202-03-01</t>
+          <t>211-01</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1246,32 +1290,34 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>rappi</t>
+          <t>provisióndeimsspatronalporpagar</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>21081.23</v>
+        <v>8540.969999999999</v>
       </c>
       <c r="E19" t="n">
-        <v>4465109.05</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>4663044.94</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>219017.12</v>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>CUENTA 202-03-01 NOMBRE rappi</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>Cuentas y documentos por pagar</t>
-        </is>
-      </c>
+        <v>8540.969999999999</v>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
+        <is>
+          <t>CUENTA 211-01 NOMBRE provisióndeimsspatronalporpagar</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Activos intangibles</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -1280,7 +1326,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>202-03-02</t>
+          <t>212-01</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1290,32 +1336,34 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>uber</t>
+          <t>provisióndeimpuestoestatalsobrenóminaporpagar</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>41830.91</v>
+        <v>12434.32</v>
       </c>
       <c r="E20" t="n">
-        <v>14028208.62</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>14371688.59</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>385310.88</v>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>CUENTA 202-03-02 NOMBRE uber</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>Cuentas y documentos por pagar</t>
-        </is>
-      </c>
+        <v>12434.32</v>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
+        <is>
+          <t>CUENTA 212-01 NOMBRE provisióndeimpuestoestatalsobrenóminaporpagar</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Activos intangibles</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -1324,7 +1372,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>205-01</t>
+          <t>213-01</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1334,32 +1382,34 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>socios accionistas o representante legal</t>
+          <t>ivaporpagar</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>36205.45</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>6665.89</v>
       </c>
       <c r="G21" t="n">
-        <v>36205.45</v>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>CUENTA 205-01 NOMBRE socios accionistas o representante legal</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>Acreedores diversos</t>
-        </is>
-      </c>
+        <v>6665.89</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
+        <is>
+          <t>CUENTA 213-01 NOMBRE ivaporpagar</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Ganancia cambiaria</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -1368,7 +1418,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>205-01-001</t>
+          <t>216-01</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1378,41 +1428,43 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>carry pkr holding</t>
+          <t>impuestosretenidosdeisrporsueldosysalarios</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>24499.91</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>27773</v>
       </c>
       <c r="F22" t="n">
-        <v>38126.65</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>38126.65</v>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>CUENTA 205-01-001 NOMBRE carry pkr holding</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>Acreedores diversos</t>
-        </is>
-      </c>
+        <v>-3273.09</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t>PR</t>
+          <t>CUENTA 216-01 NOMBRE impuestosretenidosdeisrporsueldosysalarios</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Activos intangibles</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>PNR</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>205-02</t>
+          <t>216-04</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1422,41 +1474,43 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>acreedores diversos a corto plazo nacional</t>
+          <t>impuestosretenidosdeisrporserviciosprofesionales</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>4500</v>
+        <v>1060</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>1060</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>4500</v>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>CUENTA 205-02 NOMBRE acreedores diversos a corto plazo nacional</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>Acreedores diversos</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
-          <t>PR</t>
+          <t>CUENTA 216-04 NOMBRE impuestosretenidosdeisrporserviciosprofesionales</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Compras netas nacionales</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>PNR</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>205-05-01</t>
+          <t>216-10</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1466,32 +1520,34 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>colombia</t>
+          <t>impuestosretenidosdeiva</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>15219.07</v>
+        <v>1130.67</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>1131</v>
       </c>
       <c r="F24" t="n">
-        <v>4630.54</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>19849.61</v>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>CUENTA 205-05-01 NOMBRE colombia</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>Acreedores diversos</t>
-        </is>
-      </c>
+        <v>-0.33</v>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr">
+        <is>
+          <t>CUENTA 216-10 NOMBRE impuestosretenidosdeiva</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Impuestos por pagar</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -1500,7 +1556,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>206-01</t>
+          <t>218-01-01</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1510,41 +1566,43 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>anticipo de cliente nacional</t>
+          <t>jeeves</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>17912.78</v>
       </c>
       <c r="E25" t="n">
-        <v>16536.61</v>
+        <v>162548.61</v>
       </c>
       <c r="F25" t="n">
-        <v>16536.61</v>
+        <v>146571.42</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>CUENTA 206-01 NOMBRE anticipo de cliente nacional</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>Anticipo de clientes</t>
-        </is>
-      </c>
+        <v>1935.59</v>
+      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
-          <t>PNR</t>
+          <t>CUENTA 218-01-01 NOMBRE jeeves</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Acreedores diversos</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>PR</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>208-01</t>
+          <t>301-01</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1554,41 +1612,43 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>iva trasladado cobrado</t>
+          <t>capitalfijo</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E26" t="n">
-        <v>1900605.56</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>1900605.56</v>
+        <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>CUENTA 208-01 NOMBRE iva trasladado cobrado</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>Impuestos por pagar</t>
-        </is>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t>PNR</t>
+          <t>CUENTA 301-01 NOMBRE capitalfijo</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Acreedores diversos</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>PR</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>209-01</t>
+          <t>301-03</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1598,41 +1658,43 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>iva trasladado no cobrado</t>
+          <t>aportacionesparafuturosaumentosdecapital</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>54268.91</v>
+        <v>3357652.18</v>
       </c>
       <c r="E27" t="n">
-        <v>1959853.37</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>1990323.68</v>
+        <v>940194.88</v>
       </c>
       <c r="G27" t="n">
-        <v>84739.22</v>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>CUENTA 209-01 NOMBRE iva trasladado no cobrado</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>Impuestos por pagar</t>
-        </is>
-      </c>
+        <v>4297847.06</v>
+      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
-          <t>PNR</t>
+          <t>CUENTA 301-03 NOMBRE aportacionesparafuturosaumentosdecapital</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Acreedores diversos</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>PR</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>213-01</t>
+          <t>304-02-01</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1642,41 +1704,43 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>iva por pagar</t>
+          <t>perdidadelejercicio2022</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>-1737887.67</v>
       </c>
       <c r="E28" t="n">
-        <v>450907.69</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>515103.73</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>64196.04</v>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>CUENTA 213-01 NOMBRE iva por pagar</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>Impuestos por pagar</t>
-        </is>
-      </c>
+        <v>-1737887.67</v>
+      </c>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
-          <t>PNR</t>
+          <t>CUENTA 304-02-01 NOMBRE perdidadelejercicio2022</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Cuentas y documentos por pagar</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>PR</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>213-03</t>
+          <t>304-02-02</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1686,41 +1750,43 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>isr por pagar</t>
+          <t>perdidadelejercicio2023</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>-1602971.73</v>
       </c>
       <c r="E29" t="n">
-        <v>3283</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>6418</v>
+        <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>3135</v>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>CUENTA 213-03 NOMBRE isr por pagar</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>Impuestos por pagar</t>
-        </is>
-      </c>
+        <v>-1602971.73</v>
+      </c>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr">
         <is>
-          <t>PNR</t>
+          <t>CUENTA 304-02-02 NOMBRE perdidadelejercicio2023</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Cuentas y documentos por pagar</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>PR</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>216-04</t>
+          <t>401-01</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1730,32 +1796,34 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>impuestos retenidos de isr por servicios profesionales</t>
+          <t>ventasyoserviciosgravadosalatasageneral</t>
         </is>
       </c>
       <c r="D30" t="n">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>4195.9</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>4195.8</v>
+        <v>328526.1</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>CUENTA 216-04 NOMBRE impuestos retenidos de isr por servicios profesionales</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>Impuestos por pagar</t>
-        </is>
-      </c>
+        <v>328526.1</v>
+      </c>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr">
+        <is>
+          <t>CUENTA 401-01 NOMBRE ventasyoserviciosgravadosalatasageneral</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Ventas y/o servicios nacionales</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -1764,42 +1832,44 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>216-10</t>
+          <t>501-01-01</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>impuestos retenidos de iva</t>
+          <t>comisiones</t>
         </is>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>4475.77</v>
+        <v>1470.55</v>
       </c>
       <c r="F31" t="n">
-        <v>4475.54</v>
+        <v>1458.92</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.23</v>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>CUENTA 216-10 NOMBRE impuestos retenidos de iva</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>Impuestos por pagar</t>
-        </is>
-      </c>
+        <v>11.63</v>
+      </c>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr">
+        <is>
+          <t>CUENTA 501-01-01 NOMBRE comisiones</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Compras netas nacionales</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -1808,7 +1878,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>218-01-001</t>
+          <t>503-01</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1818,32 +1888,34 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>propinas x pagar</t>
+          <t>devolucionesdescuentosobonificacionessobrecompras</t>
         </is>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>904865.95</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>1073390.51</v>
+        <v>8000</v>
       </c>
       <c r="G32" t="n">
-        <v>168524.56</v>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>CUENTA 218-01-001 NOMBRE propinas x pagar</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>Provisiones</t>
-        </is>
-      </c>
+        <v>8000</v>
+      </c>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr">
+        <is>
+          <t>CUENTA 503-01 NOMBRE devolucionesdescuentosobonificacionessobrecompras</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Ganancia cambiaria</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -1852,130 +1924,136 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>301-01</t>
+          <t>601-83</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>capital fijo</t>
+          <t>gastosnodeduciblessinrequisitosfiscales</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>11498.11</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>11498.11</v>
       </c>
       <c r="G33" t="n">
-        <v>100000</v>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>CUENTA 301-01 NOMBRE capital fijo</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>Capital Social</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr">
         <is>
-          <t>PR</t>
+          <t>CUENTA 601-83 NOMBRE gastosnodeduciblessinrequisitosfiscales</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Gastos de administración</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>PNR</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>301-03</t>
+          <t>602-83</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>aportaciones para futuros aumentos de capital</t>
+          <t>gastosnodeduciblessinrequisitosfiscales</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>197458</v>
+        <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>1061.26</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>197458</v>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>CUENTA 301-03 NOMBRE aportaciones para futuros aumentos de capital</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>Acreedores diversos</t>
-        </is>
-      </c>
+        <v>1061.26</v>
+      </c>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr">
         <is>
-          <t>PR</t>
+          <t>CUENTA 602-83 NOMBRE gastosnodeduciblessinrequisitosfiscales</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Gastos de administración</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>PNR</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>304-05</t>
+          <t>603-38</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>pérdida del ejercicio 2022</t>
+          <t>honorariosapersonasmoralesresidentesnacionales</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>-88962.12</v>
+        <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>8000</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>-88962.12</v>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>CUENTA 304-05 NOMBRE pérdida del ejercicio 2022</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>Pérdidas acumuladas</t>
-        </is>
-      </c>
+        <v>8000</v>
+      </c>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
+        <is>
+          <t>CUENTA 603-38 NOMBRE honorariosapersonasmoralesresidentesnacionales</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Gastos de administración</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -1984,42 +2062,44 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>304-06</t>
+          <t>603-59</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>utilidad del ejercicio 2023</t>
+          <t>recargosfiscales</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>37093.01</v>
+        <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>10211</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>37093.01</v>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>CUENTA 304-06 NOMBRE utilidad del ejercicio 2023</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>Pérdidas acumuladas</t>
-        </is>
-      </c>
+        <v>10211</v>
+      </c>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr">
+        <is>
+          <t>CUENTA 603-59 NOMBRE recargosfiscales</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Gastos de administración</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -2028,42 +2108,44 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>401-01</t>
+          <t>603-62</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ventas yo servicios gravados a la tasa general</t>
+          <t>capacitaciónalpersonal</t>
         </is>
       </c>
       <c r="D37" t="n">
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>20222.91</v>
+        <v>4000</v>
       </c>
       <c r="F37" t="n">
-        <v>12437827.75</v>
+        <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>12417604.84</v>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>CUENTA 401-01 NOMBRE ventas yo servicios gravados a la tasa general</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>Ventas y/o servicios nacionales</t>
-        </is>
-      </c>
+        <v>4000</v>
+      </c>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr">
+        <is>
+          <t>CUENTA 603-62 NOMBRE capacitaciónalpersonal</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Gastos de administración</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -2072,7 +2154,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>501-09</t>
+          <t>603-81</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2082,32 +2164,34 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>proveedores de logística</t>
+          <t>gastosnodeduciblessinrequisitosfiscales</t>
         </is>
       </c>
       <c r="D38" t="n">
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>8630344.58</v>
+        <v>1083398.54</v>
       </c>
       <c r="F38" t="n">
-        <v>273354.68</v>
+        <v>67353.14999999999</v>
       </c>
       <c r="G38" t="n">
-        <v>8356989.9</v>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>CUENTA 501-09 NOMBRE proveedores de logística</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>Compras netas nacionales</t>
-        </is>
-      </c>
+        <v>1016045.39</v>
+      </c>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr">
+        <is>
+          <t>CUENTA 603-81 NOMBRE gastosnodeduciblessinrequisitosfiscales</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Gastos de administración</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -2116,7 +2200,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>603-32</t>
+          <t>603-82</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2126,32 +2210,34 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>servicios administrativos</t>
+          <t>otrosgastosdeadministración</t>
         </is>
       </c>
       <c r="D39" t="n">
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>13300</v>
+        <v>37351.12</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>13300</v>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>CUENTA 603-32 NOMBRE servicios administrativos</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
+        <v>37351.12</v>
+      </c>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>CUENTA 603-82 NOMBRE otrosgastosdeadministración</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
         <is>
           <t>Gastos de administración</t>
         </is>
       </c>
-      <c r="J39" t="inlineStr">
+      <c r="L39" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -2160,7 +2246,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>603-34</t>
+          <t>701-01</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2170,32 +2256,34 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>honorarios a personas físicas residentes nacionales</t>
+          <t>pérdidacambiaria</t>
         </is>
       </c>
       <c r="D40" t="n">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>20979.03</v>
+        <v>20309.09</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>20979.03</v>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>CUENTA 603-34 NOMBRE honorarios a personas físicas residentes nacionales</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>Gastos de administración</t>
-        </is>
-      </c>
+        <v>20309.09</v>
+      </c>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
+        <is>
+          <t>CUENTA 701-01 NOMBRE pérdidacambiaria</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Pérdida cambiaria</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -2204,7 +2292,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>603-38</t>
+          <t>701-10</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2214,32 +2302,34 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>honorarios a personas morales residentes nacionales</t>
+          <t>comisionesbancarias</t>
         </is>
       </c>
       <c r="D41" t="n">
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>31360</v>
+        <v>3593.52</v>
       </c>
       <c r="F41" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>30360</v>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>CUENTA 603-38 NOMBRE honorarios a personas morales residentes nacionales</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr">
+        <v>3593.52</v>
+      </c>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>CUENTA 701-10 NOMBRE comisionesbancarias</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
         <is>
           <t>Gastos de administración</t>
         </is>
       </c>
-      <c r="J41" t="inlineStr">
+      <c r="L41" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -2248,42 +2338,44 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>603-46</t>
+          <t>702-01</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>arrendamiento a personas morales residentes nacionales</t>
+          <t>utilidadcambiaria</t>
         </is>
       </c>
       <c r="D42" t="n">
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>7746.4</v>
+        <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>1925.71</v>
+        <v>52084.81</v>
       </c>
       <c r="G42" t="n">
-        <v>5820.69</v>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>CUENTA 603-46 NOMBRE arrendamiento a personas morales residentes nacionales</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>Gastos de administración</t>
-        </is>
-      </c>
+        <v>52084.81</v>
+      </c>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr">
+        <is>
+          <t>CUENTA 702-01 NOMBRE utilidadcambiaria</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Ganancia cambiaria</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -2292,7 +2384,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>603-55</t>
+          <t>899-03</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2302,32 +2394,34 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>papelería y artículos de oficina</t>
+          <t>asientosnocuadrados</t>
         </is>
       </c>
       <c r="D43" t="n">
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>8925</v>
+        <v>0.01</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G43" t="n">
-        <v>8925</v>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>CUENTA 603-55 NOMBRE papelería y artículos de oficina</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>Gastos de administración</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
       <c r="J43" t="inlineStr">
+        <is>
+          <t>CUENTA 899-03 NOMBRE asientosnocuadrados</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Pérdida cambiaria</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>
@@ -2336,7 +2430,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>603-58</t>
+          <t>899-04</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2346,472 +2440,34 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>otros impuestos y derechos</t>
+          <t>traspasobancario</t>
         </is>
       </c>
       <c r="D44" t="n">
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>10206</v>
+        <v>291275.94</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>278510.9</v>
       </c>
       <c r="G44" t="n">
-        <v>10206</v>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>CUENTA 603-58 NOMBRE otros impuestos y derechos</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>Gastos de administración</t>
-        </is>
-      </c>
+        <v>12765.04</v>
+      </c>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr">
         <is>
-          <t>PNR</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>603-59</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>recargos fiscales</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" t="n">
-        <v>3.47</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" t="n">
-        <v>3.47</v>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>CUENTA 603-59 NOMBRE recargos fiscales</t>
-        </is>
-      </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>Gastos de administración</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>PNR</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>603-60</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>cuotas y suscripciones</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
-        <v>0</v>
-      </c>
-      <c r="E46" t="n">
-        <v>750</v>
-      </c>
-      <c r="F46" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" t="n">
-        <v>750</v>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>CUENTA 603-60 NOMBRE cuotas y suscripciones</t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>Gastos de administración</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>PNR</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>603-81</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>gastos no deducibles sin requisitos fiscales</t>
-        </is>
-      </c>
-      <c r="D47" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" t="n">
-        <v>149706.87</v>
-      </c>
-      <c r="F47" t="n">
-        <v>9795.690000000001</v>
-      </c>
-      <c r="G47" t="n">
-        <v>139911.18</v>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>CUENTA 603-81 NOMBRE gastos no deducibles sin requisitos fiscales</t>
-        </is>
-      </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>Gastos de administración</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>PNR</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>603-83</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>servicios contables</t>
-        </is>
-      </c>
-      <c r="D48" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" t="n">
-        <v>183285</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" t="n">
-        <v>183285</v>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>CUENTA 603-83 NOMBRE servicios contables</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>Gastos de administración</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>PNR</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>603-87</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>servicios tecnológicos pr</t>
-        </is>
-      </c>
-      <c r="D49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" t="n">
-        <v>3454551</v>
-      </c>
-      <c r="F49" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" t="n">
-        <v>3454551</v>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>CUENTA 603-87 NOMBRE servicios tecnológicos pr</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>Gastos de administración</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>PNR</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>701-01</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>pérdida cambiaria</t>
-        </is>
-      </c>
-      <c r="D50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E50" t="n">
-        <v>9440.23</v>
-      </c>
-      <c r="F50" t="n">
-        <v>0</v>
-      </c>
-      <c r="G50" t="n">
-        <v>9440.23</v>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>CUENTA 701-01 NOMBRE pérdida cambiaria</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
+          <t>CUENTA 899-04 NOMBRE traspasobancario</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
         <is>
           <t>Pérdida cambiaria</t>
         </is>
       </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>PNR</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>701-10</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>comisiones bancarias</t>
-        </is>
-      </c>
-      <c r="D51" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" t="n">
-        <v>250472.22</v>
-      </c>
-      <c r="F51" t="n">
-        <v>4741.6</v>
-      </c>
-      <c r="G51" t="n">
-        <v>245730.62</v>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>CUENTA 701-10 NOMBRE comisiones bancarias</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>Gastos financieros</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>PNR</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>702-01</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>utilidad cambiaria</t>
-        </is>
-      </c>
-      <c r="D52" t="n">
-        <v>0</v>
-      </c>
-      <c r="E52" t="n">
-        <v>0</v>
-      </c>
-      <c r="F52" t="n">
-        <v>33803.83</v>
-      </c>
-      <c r="G52" t="n">
-        <v>33803.83</v>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>CUENTA 702-01 NOMBRE utilidad cambiaria</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>Ganancia cambiaria</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>PNR</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>702-04</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>intereses a favor bancarios nacional</t>
-        </is>
-      </c>
-      <c r="D53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="G53" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>CUENTA 702-04 NOMBRE intereses a favor bancarios nacional</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>Intereses devengados a favor nacionales</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>PNR</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>899-04</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>traspaso bancario</t>
-        </is>
-      </c>
-      <c r="D54" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" t="n">
-        <v>7214974.14</v>
-      </c>
-      <c r="F54" t="n">
-        <v>7214974.14</v>
-      </c>
-      <c r="G54" t="n">
-        <v>0</v>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>CUENTA 899-04 NOMBRE traspaso bancario</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>Gastos de administración</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
+      <c r="L44" t="inlineStr">
         <is>
           <t>PNR</t>
         </is>

</xml_diff>